<commit_message>
Co-authored-by: Anto Wiranto <antowrnto11@gmail.com>
</commit_message>
<xml_diff>
--- a/storage/neraca-saldo-2022.xlsx
+++ b/storage/neraca-saldo-2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>DATA NERACA SALDO</t>
   </si>
@@ -32,13 +32,13 @@
     <t>DES 2021</t>
   </si>
   <si>
-    <t>Debet Jul 2022</t>
-  </si>
-  <si>
-    <t>Kredit Jul 2022</t>
-  </si>
-  <si>
-    <t>Saldo Jul 2022</t>
+    <t>Debet Aug 2022</t>
+  </si>
+  <si>
+    <t>Kredit Aug 2022</t>
+  </si>
+  <si>
+    <t>Saldo Aug 2022</t>
   </si>
   <si>
     <t>Selisih</t>
@@ -56,15 +56,6 @@
     <t>3,906,195,607</t>
   </si>
   <si>
-    <t>2,417,855,642</t>
-  </si>
-  <si>
-    <t>2,371,173,004</t>
-  </si>
-  <si>
-    <t>3,952,878,245</t>
-  </si>
-  <si>
     <t>ASET LANCAR</t>
   </si>
   <si>
@@ -74,45 +65,18 @@
     <t>326,700,530</t>
   </si>
   <si>
-    <t>1,520,658,205</t>
-  </si>
-  <si>
-    <t>854,422,503</t>
-  </si>
-  <si>
-    <t>992,936,232</t>
-  </si>
-  <si>
     <t>Kas PK</t>
   </si>
   <si>
     <t>4,687,041</t>
   </si>
   <si>
-    <t>173,557,020</t>
-  </si>
-  <si>
-    <t>177,000,000</t>
-  </si>
-  <si>
-    <t>1,244,061</t>
-  </si>
-  <si>
     <t>Mandiri</t>
   </si>
   <si>
     <t>213,381,865</t>
   </si>
   <si>
-    <t>134,268,196</t>
-  </si>
-  <si>
-    <t>513,806</t>
-  </si>
-  <si>
-    <t>347,136,255</t>
-  </si>
-  <si>
     <t>Bank BL</t>
   </si>
   <si>
@@ -122,15 +86,6 @@
     <t>108,631,624</t>
   </si>
   <si>
-    <t>1,212,832,989</t>
-  </si>
-  <si>
-    <t>676,908,697</t>
-  </si>
-  <si>
-    <t>644,555,916</t>
-  </si>
-  <si>
     <t>Kas Bank Yang Dibatasi Penggunaanya</t>
   </si>
   <si>
@@ -140,123 +95,54 @@
     <t>3,579,495,077</t>
   </si>
   <si>
-    <t>897,197,437</t>
-  </si>
-  <si>
-    <t>1,516,750,501</t>
-  </si>
-  <si>
-    <t>2,959,942,013</t>
-  </si>
-  <si>
     <t>Piutang Mitra Binaan</t>
   </si>
   <si>
     <t>4,887,807,520</t>
   </si>
   <si>
-    <t>675,000,000</t>
-  </si>
-  <si>
-    <t>1,220,551,007</t>
-  </si>
-  <si>
-    <t>4,342,256,513</t>
-  </si>
-  <si>
     <t>Sektor Industri</t>
   </si>
   <si>
     <t>810,118,000</t>
   </si>
   <si>
-    <t>220,000,000</t>
-  </si>
-  <si>
-    <t>223,875,000</t>
-  </si>
-  <si>
-    <t>806,243,000</t>
-  </si>
-  <si>
     <t>Sektor Perdagangan</t>
   </si>
   <si>
     <t>2,590,816,860</t>
   </si>
   <si>
-    <t>315,000,000</t>
-  </si>
-  <si>
-    <t>665,509,007</t>
-  </si>
-  <si>
-    <t>2,240,307,853</t>
-  </si>
-  <si>
     <t>Sektor Pertanian</t>
   </si>
   <si>
     <t>231,074,500</t>
   </si>
   <si>
-    <t>80,272,500</t>
-  </si>
-  <si>
-    <t>150,802,000</t>
-  </si>
-  <si>
     <t>Sektor Perkebunan</t>
   </si>
   <si>
     <t>50,416,000</t>
   </si>
   <si>
-    <t>4,309,000</t>
-  </si>
-  <si>
-    <t>46,107,000</t>
-  </si>
-  <si>
     <t>Sektor Perikanan</t>
   </si>
   <si>
     <t>230,316,640</t>
   </si>
   <si>
-    <t>42,543,000</t>
-  </si>
-  <si>
-    <t>187,773,640</t>
-  </si>
-  <si>
     <t>Sektor Peternakan</t>
   </si>
   <si>
     <t>364,927,520</t>
   </si>
   <si>
-    <t>18,686,500</t>
-  </si>
-  <si>
-    <t>346,241,020</t>
-  </si>
-  <si>
     <t>Sektor Jasa</t>
   </si>
   <si>
     <t>594,472,000</t>
   </si>
   <si>
-    <t>140,000,000</t>
-  </si>
-  <si>
-    <t>185,356,000</t>
-  </si>
-  <si>
-    <t>549,116,000</t>
-  </si>
-  <si>
     <t>Sektor Lain-Lain</t>
   </si>
   <si>
@@ -269,99 +155,27 @@
     <t>-1,308,312,443</t>
   </si>
   <si>
-    <t>211,142,117</t>
-  </si>
-  <si>
-    <t>285,144,174</t>
-  </si>
-  <si>
-    <t>-1,382,314,500</t>
-  </si>
-  <si>
     <t>-235,581,986</t>
   </si>
   <si>
-    <t>12,093,881</t>
-  </si>
-  <si>
-    <t>32,879,152</t>
-  </si>
-  <si>
-    <t>-256,367,257</t>
-  </si>
-  <si>
     <t>-766,086,864</t>
   </si>
   <si>
-    <t>144,888,481</t>
-  </si>
-  <si>
-    <t>87,896,840</t>
-  </si>
-  <si>
-    <t>-709,095,223</t>
-  </si>
-  <si>
     <t>-27,129,394</t>
   </si>
   <si>
-    <t>3,723,882</t>
-  </si>
-  <si>
-    <t>1,918,995</t>
-  </si>
-  <si>
-    <t>-25,324,507</t>
-  </si>
-  <si>
     <t>-1,599,041</t>
   </si>
   <si>
-    <t>771,402</t>
-  </si>
-  <si>
-    <t>717,272</t>
-  </si>
-  <si>
-    <t>-1,544,911</t>
-  </si>
-  <si>
     <t>-39,489,349</t>
   </si>
   <si>
-    <t>2,861,973</t>
-  </si>
-  <si>
-    <t>6,219,498</t>
-  </si>
-  <si>
-    <t>-42,846,874</t>
-  </si>
-  <si>
     <t>-175,998,033</t>
   </si>
   <si>
-    <t>7,165,050</t>
-  </si>
-  <si>
-    <t>50,026,550</t>
-  </si>
-  <si>
-    <t>-218,859,533</t>
-  </si>
-  <si>
     <t>-46,761,776</t>
   </si>
   <si>
-    <t>39,637,448</t>
-  </si>
-  <si>
-    <t>105,485,867</t>
-  </si>
-  <si>
-    <t>-112,610,195</t>
-  </si>
-  <si>
     <t>-15,666,000</t>
   </si>
   <si>
@@ -371,33 +185,12 @@
     <t>4,316,437,323</t>
   </si>
   <si>
-    <t>377,500</t>
-  </si>
-  <si>
-    <t>10,677,820</t>
-  </si>
-  <si>
-    <t>4,306,137,003</t>
-  </si>
-  <si>
     <t>2,101,653,303</t>
   </si>
   <si>
-    <t>1,937,500</t>
-  </si>
-  <si>
-    <t>2,100,093,303</t>
-  </si>
-  <si>
     <t>419,765,962</t>
   </si>
   <si>
-    <t>6,298,000</t>
-  </si>
-  <si>
-    <t>413,467,962</t>
-  </si>
-  <si>
     <t>273,800,650</t>
   </si>
   <si>
@@ -410,33 +203,18 @@
     <t>1,445,242,108</t>
   </si>
   <si>
-    <t>2,442,320</t>
-  </si>
-  <si>
-    <t>1,442,799,788</t>
-  </si>
-  <si>
     <t>2. Alokasi Penyisihan Piutang Bermasalah</t>
   </si>
   <si>
     <t>-4,316,437,323</t>
   </si>
   <si>
-    <t>-4,306,137,003</t>
-  </si>
-  <si>
     <t>-2,101,653,303</t>
   </si>
   <si>
-    <t>-2,100,093,303</t>
-  </si>
-  <si>
     <t>-419,765,962</t>
   </si>
   <si>
-    <t>-413,467,962</t>
-  </si>
-  <si>
     <t>-273,800,650</t>
   </si>
   <si>
@@ -449,9 +227,6 @@
     <t>-1,445,242,108</t>
   </si>
   <si>
-    <t>-1,442,799,788</t>
-  </si>
-  <si>
     <t>Piutang Jasa Adm Pinjaman</t>
   </si>
   <si>
@@ -476,27 +251,12 @@
     <t>3,906,195,606</t>
   </si>
   <si>
-    <t>289,657,206</t>
-  </si>
-  <si>
-    <t>336,339,844</t>
-  </si>
-  <si>
-    <t>3,952,878,244</t>
-  </si>
-  <si>
     <t>Liabilitas</t>
   </si>
   <si>
     <t>135,922,648</t>
   </si>
   <si>
-    <t>1,552,710</t>
-  </si>
-  <si>
-    <t>137,475,358</t>
-  </si>
-  <si>
     <t>Liabilitas Jangka Pendek</t>
   </si>
   <si>
@@ -506,9 +266,6 @@
     <t>3,075,060</t>
   </si>
   <si>
-    <t>4,627,770</t>
-  </si>
-  <si>
     <t>2. Angsuran Belum Teridentifikasi</t>
   </si>
   <si>
@@ -521,72 +278,36 @@
     <t>3,770,272,958</t>
   </si>
   <si>
-    <t>334,787,134</t>
-  </si>
-  <si>
-    <t>3,815,402,886</t>
-  </si>
-  <si>
     <t>Aktiva Bersih Awal Periode</t>
   </si>
   <si>
     <t>3,488,933,969</t>
   </si>
   <si>
-    <t>-289,336,566</t>
-  </si>
-  <si>
-    <t>-108,852,738</t>
-  </si>
-  <si>
-    <t>3,308,450,141</t>
-  </si>
-  <si>
     <t>Pendapatan</t>
   </si>
   <si>
     <t>342,652,403</t>
   </si>
   <si>
-    <t>160,320</t>
-  </si>
-  <si>
-    <t>112,967,198</t>
-  </si>
-  <si>
-    <t>112,806,878</t>
-  </si>
-  <si>
     <t>Jasa Administrasi Pinjaman</t>
   </si>
   <si>
     <t>147,692,944</t>
   </si>
   <si>
-    <t>107,782,180</t>
-  </si>
-  <si>
-    <t>107,621,860</t>
-  </si>
-  <si>
     <t>Jasa Giro PK</t>
   </si>
   <si>
     <t>7,280,735</t>
   </si>
   <si>
-    <t>4,185,018</t>
-  </si>
-  <si>
     <t>Pendapatan Lain-Lain, Piutang Hap</t>
   </si>
   <si>
     <t>21,678,300</t>
   </si>
   <si>
-    <t>1,000,000</t>
-  </si>
-  <si>
     <t>Pendapatan Lain-Lain, Lain-Lain</t>
   </si>
   <si>
@@ -599,12 +320,6 @@
     <t>-4,176,647</t>
   </si>
   <si>
-    <t>2,422,503</t>
-  </si>
-  <si>
-    <t>-2,422,503</t>
-  </si>
-  <si>
     <t>Beban Adm dan Umum</t>
   </si>
   <si>
@@ -614,76 +329,28 @@
     <t>-53,887,934</t>
   </si>
   <si>
-    <t>285,521,675</t>
-  </si>
-  <si>
-    <t>221,819,936</t>
-  </si>
-  <si>
-    <t>-63,701,737</t>
-  </si>
-  <si>
     <t>-94,289,373</t>
   </si>
   <si>
-    <t>33,256,652</t>
-  </si>
-  <si>
-    <t>14,031,381</t>
-  </si>
-  <si>
-    <t>-19,225,271</t>
-  </si>
-  <si>
     <t>-15,725,775</t>
   </si>
   <si>
-    <t>151,186,481</t>
-  </si>
-  <si>
-    <t>63,289,641</t>
-  </si>
-  <si>
     <t>6,973,100</t>
   </si>
   <si>
-    <t>1,804,887</t>
-  </si>
-  <si>
-    <t>54,130</t>
-  </si>
-  <si>
     <t>41,935,073</t>
   </si>
   <si>
-    <t>-3,357,525</t>
-  </si>
-  <si>
     <t>-19,438,118</t>
   </si>
   <si>
-    <t>-42,861,500</t>
-  </si>
-  <si>
     <t>28,256,200</t>
   </si>
   <si>
-    <t>42,079,768</t>
-  </si>
-  <si>
-    <t>-63,406,099</t>
-  </si>
-  <si>
     <t>Beban Lain-Lain</t>
   </si>
   <si>
     <t>-3,248,833</t>
-  </si>
-  <si>
-    <t>1,552,708</t>
-  </si>
-  <si>
-    <t>-1,552,708</t>
   </si>
   <si>
     <t>Lain-Lain</t>
@@ -1129,14 +796,14 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1150,19 +817,19 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1176,19 +843,19 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1202,19 +869,19 @@
         <v>101010101</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1228,19 +895,19 @@
         <v>101010201</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1254,7 +921,7 @@
         <v>101010202</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1280,19 +947,19 @@
         <v>101010204</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1306,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1332,7 +999,7 @@
         <v>103070000</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1358,19 +1025,19 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1384,19 +1051,19 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" t="s">
-        <v>48</v>
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1410,19 +1077,19 @@
         <v>101060100</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1436,19 +1103,19 @@
         <v>101060200</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" t="s">
-        <v>58</v>
+        <v>31</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1462,19 +1129,19 @@
         <v>101060300</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" t="s">
-        <v>62</v>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1488,19 +1155,19 @@
         <v>101060400</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" t="s">
-        <v>66</v>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1514,19 +1181,19 @@
         <v>101060500</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1540,19 +1207,19 @@
         <v>101060600</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" t="s">
-        <v>74</v>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1566,19 +1233,19 @@
         <v>101060700</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>79</v>
+        <v>41</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1592,10 +1259,10 @@
         <v>101060800</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1603,8 +1270,8 @@
       <c r="F23">
         <v>0</v>
       </c>
-      <c r="G23" t="s">
-        <v>81</v>
+      <c r="G23">
+        <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1618,19 +1285,19 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" t="s">
-        <v>86</v>
+        <v>45</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1644,19 +1311,19 @@
         <v>101070100</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" t="s">
-        <v>89</v>
-      </c>
-      <c r="G25" t="s">
-        <v>90</v>
+        <v>46</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1670,19 +1337,19 @@
         <v>101070200</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" t="s">
-        <v>93</v>
-      </c>
-      <c r="G26" t="s">
-        <v>94</v>
+        <v>47</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1696,19 +1363,19 @@
         <v>101070300</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" t="s">
-        <v>98</v>
+        <v>48</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1722,19 +1389,19 @@
         <v>101070400</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" t="s">
-        <v>102</v>
+        <v>49</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1748,19 +1415,19 @@
         <v>101070500</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" t="s">
-        <v>105</v>
-      </c>
-      <c r="G29" t="s">
-        <v>106</v>
+        <v>50</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -1774,19 +1441,19 @@
         <v>101070600</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" t="s">
-        <v>109</v>
-      </c>
-      <c r="G30" t="s">
-        <v>110</v>
+        <v>51</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1800,19 +1467,19 @@
         <v>101070700</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" t="s">
-        <v>112</v>
-      </c>
-      <c r="F31" t="s">
-        <v>113</v>
-      </c>
-      <c r="G31" t="s">
-        <v>114</v>
+        <v>52</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1826,10 +1493,10 @@
         <v>101070800</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1837,8 +1504,8 @@
       <c r="F32">
         <v>0</v>
       </c>
-      <c r="G32" t="s">
-        <v>115</v>
+      <c r="G32">
+        <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1852,19 +1519,19 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" t="s">
-        <v>120</v>
+        <v>55</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
       </c>
       <c r="H33">
         <v>1234</v>
@@ -1878,19 +1545,19 @@
         <v>103040100</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" t="s">
-        <v>122</v>
-      </c>
-      <c r="G34" t="s">
-        <v>123</v>
+        <v>56</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -1904,19 +1571,19 @@
         <v>103040200</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35" t="s">
-        <v>125</v>
-      </c>
-      <c r="G35" t="s">
-        <v>126</v>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -1930,10 +1597,10 @@
         <v>103040300</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1941,8 +1608,8 @@
       <c r="F36">
         <v>0</v>
       </c>
-      <c r="G36" t="s">
-        <v>127</v>
+      <c r="G36">
+        <v>0</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -1956,7 +1623,7 @@
         <v>103040400</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1982,10 +1649,10 @@
         <v>103040500</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1993,8 +1660,8 @@
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="G38" t="s">
-        <v>128</v>
+      <c r="G38">
+        <v>0</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2008,10 +1675,10 @@
         <v>103040600</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2019,8 +1686,8 @@
       <c r="F39">
         <v>0</v>
       </c>
-      <c r="G39" t="s">
-        <v>129</v>
+      <c r="G39">
+        <v>0</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2034,19 +1701,19 @@
         <v>103040700</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>130</v>
+        <v>61</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40" t="s">
-        <v>131</v>
-      </c>
-      <c r="G40" t="s">
-        <v>132</v>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
       </c>
       <c r="H40">
         <v>1234</v>
@@ -2060,7 +1727,7 @@
         <v>103040800</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -2086,19 +1753,19 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="D42" t="s">
-        <v>134</v>
-      </c>
-      <c r="E42" t="s">
-        <v>119</v>
-      </c>
-      <c r="F42" t="s">
-        <v>118</v>
-      </c>
-      <c r="G42" t="s">
-        <v>135</v>
+        <v>63</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
       </c>
       <c r="H42">
         <v>-1234</v>
@@ -2112,19 +1779,19 @@
         <v>103050100</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
-      </c>
-      <c r="E43" t="s">
-        <v>122</v>
-      </c>
-      <c r="F43" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" t="s">
-        <v>137</v>
+        <v>64</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2138,19 +1805,19 @@
         <v>103050200</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>138</v>
-      </c>
-      <c r="E44" t="s">
-        <v>125</v>
+        <v>65</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
       </c>
       <c r="F44">
         <v>0</v>
       </c>
-      <c r="G44" t="s">
-        <v>139</v>
+      <c r="G44">
+        <v>0</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -2164,10 +1831,10 @@
         <v>103050300</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2175,8 +1842,8 @@
       <c r="F45">
         <v>0</v>
       </c>
-      <c r="G45" t="s">
-        <v>140</v>
+      <c r="G45">
+        <v>0</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -2190,7 +1857,7 @@
         <v>103050400</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -2216,19 +1883,19 @@
         <v>103050500</v>
       </c>
       <c r="C47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" t="s">
         <v>67</v>
       </c>
-      <c r="D47" t="s">
-        <v>141</v>
-      </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
-      <c r="G47" t="s">
-        <v>141</v>
+      <c r="G47">
+        <v>0</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2242,10 +1909,10 @@
         <v>103050600</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2253,8 +1920,8 @@
       <c r="F48">
         <v>0</v>
       </c>
-      <c r="G48" t="s">
-        <v>142</v>
+      <c r="G48">
+        <v>0</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -2268,19 +1935,19 @@
         <v>103050700</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" t="s">
-        <v>131</v>
+        <v>69</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
-      <c r="G49" t="s">
-        <v>144</v>
+      <c r="G49">
+        <v>0</v>
       </c>
       <c r="H49">
         <v>-1234</v>
@@ -2294,7 +1961,7 @@
         <v>103050800</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -2320,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2346,7 +2013,7 @@
         <v>101080000</v>
       </c>
       <c r="C52" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2372,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -2398,10 +2065,10 @@
         <v>102010201</v>
       </c>
       <c r="C54" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="D54" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2424,10 +2091,10 @@
         <v>0</v>
       </c>
       <c r="C55" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -2450,10 +2117,10 @@
         <v>102020201</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="D56" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -2476,19 +2143,19 @@
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>151</v>
+        <v>76</v>
       </c>
       <c r="D57" t="s">
-        <v>152</v>
-      </c>
-      <c r="E57" t="s">
-        <v>153</v>
-      </c>
-      <c r="F57" t="s">
-        <v>154</v>
-      </c>
-      <c r="G57" t="s">
-        <v>155</v>
+        <v>77</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -2502,19 +2169,19 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="D58" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58" t="s">
-        <v>158</v>
-      </c>
-      <c r="G58" t="s">
-        <v>159</v>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -2528,19 +2195,19 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="D59" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59" t="s">
-        <v>158</v>
-      </c>
-      <c r="G59" t="s">
-        <v>159</v>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2554,19 +2221,19 @@
         <v>201040000</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>81</v>
       </c>
       <c r="D60" t="s">
-        <v>162</v>
+        <v>82</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60" t="s">
-        <v>158</v>
-      </c>
-      <c r="G60" t="s">
-        <v>163</v>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
       </c>
       <c r="H60">
         <v>-5486</v>
@@ -2580,10 +2247,10 @@
         <v>201050000</v>
       </c>
       <c r="C61" t="s">
-        <v>164</v>
+        <v>83</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>84</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -2591,8 +2258,8 @@
       <c r="F61">
         <v>0</v>
       </c>
-      <c r="G61" t="s">
-        <v>165</v>
+      <c r="G61">
+        <v>0</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -2606,19 +2273,19 @@
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>166</v>
+        <v>85</v>
       </c>
       <c r="D62" t="s">
-        <v>167</v>
-      </c>
-      <c r="E62" t="s">
-        <v>153</v>
-      </c>
-      <c r="F62" t="s">
-        <v>168</v>
-      </c>
-      <c r="G62" t="s">
-        <v>169</v>
+        <v>86</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
       </c>
       <c r="H62">
         <v>-1234</v>
@@ -2632,19 +2299,19 @@
         <v>400000000</v>
       </c>
       <c r="C63" t="s">
-        <v>170</v>
+        <v>87</v>
       </c>
       <c r="D63" t="s">
-        <v>171</v>
-      </c>
-      <c r="E63" t="s">
-        <v>172</v>
-      </c>
-      <c r="F63" t="s">
-        <v>173</v>
-      </c>
-      <c r="G63" t="s">
-        <v>174</v>
+        <v>88</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -2658,19 +2325,19 @@
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="D64" t="s">
-        <v>176</v>
-      </c>
-      <c r="E64" t="s">
-        <v>177</v>
-      </c>
-      <c r="F64" t="s">
-        <v>178</v>
-      </c>
-      <c r="G64" t="s">
-        <v>179</v>
+        <v>90</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2684,19 +2351,19 @@
         <v>403010100</v>
       </c>
       <c r="C65" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="D65" t="s">
-        <v>181</v>
-      </c>
-      <c r="E65" t="s">
-        <v>177</v>
-      </c>
-      <c r="F65" t="s">
-        <v>182</v>
-      </c>
-      <c r="G65" t="s">
-        <v>183</v>
+        <v>92</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -2710,19 +2377,19 @@
         <v>403020100</v>
       </c>
       <c r="C66" t="s">
-        <v>184</v>
+        <v>93</v>
       </c>
       <c r="D66" t="s">
-        <v>185</v>
+        <v>94</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
-      <c r="F66" t="s">
-        <v>186</v>
-      </c>
-      <c r="G66" t="s">
-        <v>186</v>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -2736,19 +2403,19 @@
         <v>403030100</v>
       </c>
       <c r="C67" t="s">
-        <v>187</v>
+        <v>95</v>
       </c>
       <c r="D67" t="s">
-        <v>188</v>
+        <v>96</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
-      <c r="F67" t="s">
-        <v>189</v>
-      </c>
-      <c r="G67" t="s">
-        <v>189</v>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -2788,10 +2455,10 @@
         <v>403030400</v>
       </c>
       <c r="C69" t="s">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="D69" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2814,19 +2481,19 @@
         <v>0</v>
       </c>
       <c r="C70" t="s">
-        <v>192</v>
+        <v>99</v>
       </c>
       <c r="D70" t="s">
-        <v>193</v>
-      </c>
-      <c r="E70" t="s">
-        <v>194</v>
+        <v>100</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
-      <c r="G70" t="s">
-        <v>195</v>
+      <c r="G70">
+        <v>0</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -2840,19 +2507,19 @@
         <v>407010000</v>
       </c>
       <c r="C71" t="s">
-        <v>196</v>
+        <v>101</v>
       </c>
       <c r="D71" t="s">
-        <v>193</v>
-      </c>
-      <c r="E71" t="s">
-        <v>194</v>
+        <v>100</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
-      <c r="G71" t="s">
-        <v>195</v>
+      <c r="G71">
+        <v>0</v>
       </c>
       <c r="H71">
         <v>-1234</v>
@@ -2866,19 +2533,19 @@
         <v>0</v>
       </c>
       <c r="C72" t="s">
-        <v>197</v>
+        <v>102</v>
       </c>
       <c r="D72" t="s">
-        <v>198</v>
-      </c>
-      <c r="E72" t="s">
-        <v>199</v>
-      </c>
-      <c r="F72" t="s">
-        <v>200</v>
-      </c>
-      <c r="G72" t="s">
-        <v>201</v>
+        <v>103</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -2892,19 +2559,19 @@
         <v>410010100</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D73" t="s">
-        <v>202</v>
-      </c>
-      <c r="E73" t="s">
-        <v>203</v>
-      </c>
-      <c r="F73" t="s">
-        <v>204</v>
-      </c>
-      <c r="G73" t="s">
-        <v>205</v>
+        <v>104</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -2918,19 +2585,19 @@
         <v>410020200</v>
       </c>
       <c r="C74" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D74" t="s">
-        <v>206</v>
-      </c>
-      <c r="E74" t="s">
-        <v>93</v>
-      </c>
-      <c r="F74" t="s">
-        <v>207</v>
-      </c>
-      <c r="G74" t="s">
-        <v>208</v>
+        <v>105</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -2944,19 +2611,19 @@
         <v>410030300</v>
       </c>
       <c r="C75" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D75" t="s">
-        <v>209</v>
-      </c>
-      <c r="E75" t="s">
-        <v>97</v>
-      </c>
-      <c r="F75" t="s">
-        <v>96</v>
-      </c>
-      <c r="G75" t="s">
-        <v>210</v>
+        <v>106</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -2970,19 +2637,19 @@
         <v>410040400</v>
       </c>
       <c r="C76" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D76" t="s">
-        <v>99</v>
-      </c>
-      <c r="E76" t="s">
-        <v>101</v>
-      </c>
-      <c r="F76" t="s">
-        <v>100</v>
-      </c>
-      <c r="G76" t="s">
-        <v>211</v>
+        <v>49</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -2996,19 +2663,19 @@
         <v>410050500</v>
       </c>
       <c r="C77" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D77" t="s">
-        <v>212</v>
-      </c>
-      <c r="E77" t="s">
-        <v>105</v>
-      </c>
-      <c r="F77" t="s">
-        <v>104</v>
-      </c>
-      <c r="G77" t="s">
-        <v>213</v>
+        <v>107</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3022,19 +2689,19 @@
         <v>410060600</v>
       </c>
       <c r="C78" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D78" t="s">
-        <v>214</v>
-      </c>
-      <c r="E78" t="s">
-        <v>109</v>
-      </c>
-      <c r="F78" t="s">
         <v>108</v>
       </c>
-      <c r="G78" t="s">
-        <v>215</v>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
       </c>
       <c r="H78">
         <v>-1234</v>
@@ -3048,19 +2715,19 @@
         <v>410070700</v>
       </c>
       <c r="C79" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="D79" t="s">
-        <v>216</v>
-      </c>
-      <c r="E79" t="s">
-        <v>113</v>
-      </c>
-      <c r="F79" t="s">
-        <v>217</v>
-      </c>
-      <c r="G79" t="s">
-        <v>218</v>
+        <v>109</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -3074,7 +2741,7 @@
         <v>410070700</v>
       </c>
       <c r="C80" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -3100,19 +2767,19 @@
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>219</v>
+        <v>110</v>
       </c>
       <c r="D81" t="s">
-        <v>220</v>
-      </c>
-      <c r="E81" t="s">
-        <v>221</v>
+        <v>111</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
       </c>
       <c r="F81">
         <v>0</v>
       </c>
-      <c r="G81" t="s">
-        <v>222</v>
+      <c r="G81">
+        <v>0</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -3126,19 +2793,19 @@
         <v>412010000</v>
       </c>
       <c r="C82" t="s">
-        <v>223</v>
+        <v>112</v>
       </c>
       <c r="D82" t="s">
-        <v>220</v>
-      </c>
-      <c r="E82" t="s">
-        <v>221</v>
+        <v>111</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
       </c>
       <c r="F82">
         <v>0</v>
       </c>
-      <c r="G82" t="s">
-        <v>222</v>
+      <c r="G82">
+        <v>0</v>
       </c>
       <c r="H82">
         <v>0</v>

</xml_diff>